<commit_message>
added 2018 draft and fixed/filled data
</commit_message>
<xml_diff>
--- a/data/activeStats.xlsx
+++ b/data/activeStats.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10514"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victornorris/Code/projects/gatsbyTraining/crashCourse/mlModels/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB82452-CC9F-494E-B7B5-997129C477D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="760" windowWidth="30000" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t>Name</t>
   </si>
@@ -88,6 +82,12 @@
     <t>yrs</t>
   </si>
   <si>
+    <t>A.J. Brown</t>
+  </si>
+  <si>
+    <t>Andy Isabella</t>
+  </si>
+  <si>
     <t>Antonio Gandy-Golden</t>
   </si>
   <si>
@@ -106,9 +106,18 @@
     <t>Collin Johnson</t>
   </si>
   <si>
+    <t>D.K. Metcalf</t>
+  </si>
+  <si>
+    <t>Darius Slayton</t>
+  </si>
+  <si>
     <t>Darnell Mooney</t>
   </si>
   <si>
+    <t>Deebo Samuel</t>
+  </si>
+  <si>
     <t>Denzel Mims</t>
   </si>
   <si>
@@ -118,6 +127,9 @@
     <t>Dezmon Patmon</t>
   </si>
   <si>
+    <t>Diontae Johnson</t>
+  </si>
+  <si>
     <t>Donovan Peoples-Jones</t>
   </si>
   <si>
@@ -127,9 +139,18 @@
     <t>Gabriel Davis</t>
   </si>
   <si>
+    <t>Gary Jennings Jr</t>
+  </si>
+  <si>
+    <t>Hakeem Butler</t>
+  </si>
+  <si>
     <t>Henry Ruggs III</t>
   </si>
   <si>
+    <t>Hunter Renfrow</t>
+  </si>
+  <si>
     <t>Isaiah Hodgins</t>
   </si>
   <si>
@@ -145,21 +166,36 @@
     <t>Jerry Jeudy</t>
   </si>
   <si>
+    <t>JJ Arcega-Whiteside</t>
+  </si>
+  <si>
     <t>Joe Reed</t>
   </si>
   <si>
     <t>John Hightower</t>
   </si>
   <si>
+    <t>John Ursua</t>
+  </si>
+  <si>
     <t>Justin Jefferson</t>
   </si>
   <si>
+    <t>Juwann Winfree</t>
+  </si>
+  <si>
     <t>K.J. Hill</t>
   </si>
   <si>
     <t>K.J. Osborn</t>
   </si>
   <si>
+    <t>KeeSean Johnson</t>
+  </si>
+  <si>
+    <t>Kelvin Harmon</t>
+  </si>
+  <si>
     <t>KJ Hamler</t>
   </si>
   <si>
@@ -169,104 +205,149 @@
     <t>Lynn Bowden Jr.</t>
   </si>
   <si>
+    <t>Marquise Brown</t>
+  </si>
+  <si>
+    <t>Mecole Hardman</t>
+  </si>
+  <si>
     <t>Michael Pittman Jr.</t>
   </si>
   <si>
+    <t>Miles Boykin</t>
+  </si>
+  <si>
+    <t>N'Keal Harry</t>
+  </si>
+  <si>
+    <t>Olabisi Johnson</t>
+  </si>
+  <si>
+    <t>Parris Campbell</t>
+  </si>
+  <si>
     <t>Quez Watkins</t>
   </si>
   <si>
     <t>Quintez Cephus</t>
   </si>
   <si>
+    <t>Riley Ridley</t>
+  </si>
+  <si>
+    <t>Scott Miller</t>
+  </si>
+  <si>
     <t>Tee Higgins</t>
   </si>
   <si>
+    <t>Terry Godwin</t>
+  </si>
+  <si>
+    <t>Terry McLaurin</t>
+  </si>
+  <si>
+    <t>Travis Fulgham</t>
+  </si>
+  <si>
     <t>Tyler Johnson</t>
   </si>
   <si>
     <t>Van Jefferson</t>
   </si>
   <si>
-    <t>Olabisi Johnson</t>
-  </si>
-  <si>
-    <t>Terry Godwin</t>
-  </si>
-  <si>
-    <t>John Ursua</t>
-  </si>
-  <si>
-    <t>Scott Miller</t>
-  </si>
-  <si>
-    <t>Kelvin Harmon</t>
-  </si>
-  <si>
-    <t>Juwann Winfree</t>
-  </si>
-  <si>
-    <t>Travis Fulgham</t>
-  </si>
-  <si>
-    <t>KeeSean Johnson</t>
-  </si>
-  <si>
-    <t>Darius Slayton</t>
-  </si>
-  <si>
-    <t>Hunter Renfrow</t>
-  </si>
-  <si>
-    <t>Riley Ridley</t>
-  </si>
-  <si>
-    <t>Gary Jennings Jr</t>
-  </si>
-  <si>
-    <t>Hakeem Butler</t>
-  </si>
-  <si>
-    <t>Miles Boykin</t>
-  </si>
-  <si>
-    <t>Terry McLaurin</t>
-  </si>
-  <si>
-    <t>Diontae Johnson</t>
-  </si>
-  <si>
-    <t>D.K. Metcalf</t>
-  </si>
-  <si>
-    <t>Andy Isabella</t>
-  </si>
-  <si>
-    <t>Parris Campbell</t>
-  </si>
-  <si>
-    <t>JJ Arcega-Whiteside</t>
-  </si>
-  <si>
-    <t>Mecole Hardman</t>
-  </si>
-  <si>
-    <t>A.J. Brown</t>
-  </si>
-  <si>
-    <t>Deebo Samuel</t>
-  </si>
-  <si>
-    <t>N'Keal Harry</t>
-  </si>
-  <si>
-    <t>Marquise Brown</t>
+    <t>J'Mon Moore</t>
+  </si>
+  <si>
+    <t>Jaleeel Scott</t>
+  </si>
+  <si>
+    <t>DaeSean Hamilton</t>
+  </si>
+  <si>
+    <t>Antonio Callaway</t>
+  </si>
+  <si>
+    <t>Keke Coutee</t>
+  </si>
+  <si>
+    <t>Tre'Quan Smith</t>
+  </si>
+  <si>
+    <t>Michael Gallup</t>
+  </si>
+  <si>
+    <t>DJ Chark</t>
+  </si>
+  <si>
+    <t>James Washington</t>
+  </si>
+  <si>
+    <t>Anthony Miller</t>
+  </si>
+  <si>
+    <t>Christian Kirk</t>
+  </si>
+  <si>
+    <t>Dante Pettis</t>
+  </si>
+  <si>
+    <t>Courtland Sutton</t>
+  </si>
+  <si>
+    <t>Calvin Ridley</t>
+  </si>
+  <si>
+    <t>D.J. Moore</t>
+  </si>
+  <si>
+    <t>Trey Quinn</t>
+  </si>
+  <si>
+    <t>Auden Tate</t>
+  </si>
+  <si>
+    <t>Richie James</t>
+  </si>
+  <si>
+    <t>Marcel Ateman</t>
+  </si>
+  <si>
+    <t>Javon Wims</t>
+  </si>
+  <si>
+    <t>Braxton Berrios</t>
+  </si>
+  <si>
+    <t>Cedric Wilson</t>
+  </si>
+  <si>
+    <t>Equanimeous St. Brown</t>
+  </si>
+  <si>
+    <t>Russel Gage</t>
+  </si>
+  <si>
+    <t>Ray-Ray McCloud</t>
+  </si>
+  <si>
+    <t>Deon Cain</t>
+  </si>
+  <si>
+    <t>Marquez Valdez-Scantling</t>
+  </si>
+  <si>
+    <t>Justin Watson</t>
+  </si>
+  <si>
+    <t>Allen Lazard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,21 +410,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -381,7 +454,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -415,7 +488,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -450,10 +522,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -626,16 +697,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:W88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -706,9 +775,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>2019</v>
@@ -771,9 +840,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>2019</v>
@@ -785,7 +854,7 @@
         <v>175.26</v>
       </c>
       <c r="E3">
-        <v>85.275295999999997</v>
+        <v>85.275296</v>
       </c>
       <c r="F3">
         <v>231</v>
@@ -803,7 +872,7 @@
         <v>44</v>
       </c>
       <c r="K3">
-        <v>4.3099999999999996</v>
+        <v>4.31</v>
       </c>
       <c r="L3">
         <v>36.5</v>
@@ -818,7 +887,7 @@
         <v>6.95</v>
       </c>
       <c r="P3">
-        <v>4.1500000000000004</v>
+        <v>4.15</v>
       </c>
       <c r="Q3">
         <v>62</v>
@@ -842,9 +911,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <v>2020</v>
@@ -856,7 +925,7 @@
         <v>193.04</v>
       </c>
       <c r="E4">
-        <v>45.264054542079997</v>
+        <v>45.26405454208</v>
       </c>
       <c r="F4">
         <v>150</v>
@@ -874,7 +943,7 @@
         <v>24</v>
       </c>
       <c r="K4">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="L4">
         <v>36</v>
@@ -913,9 +982,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <v>2020</v>
@@ -927,7 +996,7 @@
         <v>182.88</v>
       </c>
       <c r="E5">
-        <v>41.149140492800001</v>
+        <v>41.1491404928</v>
       </c>
       <c r="F5">
         <v>98</v>
@@ -969,9 +1038,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>2020</v>
@@ -983,7 +1052,7 @@
         <v>190.5</v>
       </c>
       <c r="E6">
-        <v>44.235326029760003</v>
+        <v>44.23532602976</v>
       </c>
       <c r="F6">
         <v>234</v>
@@ -992,7 +1061,7 @@
         <v>3045</v>
       </c>
       <c r="H6">
-        <v>13.012820512820509</v>
+        <v>13.01282051282051</v>
       </c>
       <c r="I6">
         <v>22</v>
@@ -1025,9 +1094,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>2020</v>
@@ -1039,7 +1108,7 @@
         <v>187.96</v>
       </c>
       <c r="E7">
-        <v>41.149140492800001</v>
+        <v>41.1491404928</v>
       </c>
       <c r="F7">
         <v>173</v>
@@ -1090,9 +1159,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8">
         <v>2020</v>
@@ -1104,7 +1173,7 @@
         <v>193.04</v>
       </c>
       <c r="E8">
-        <v>48.967477186431999</v>
+        <v>48.967477186432</v>
       </c>
       <c r="F8">
         <v>150</v>
@@ -1113,7 +1182,7 @@
         <v>2159</v>
       </c>
       <c r="H8">
-        <v>14.393333333333331</v>
+        <v>14.39333333333333</v>
       </c>
       <c r="I8">
         <v>19</v>
@@ -1155,9 +1224,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B9">
         <v>2020</v>
@@ -1169,7 +1238,7 @@
         <v>198.12</v>
       </c>
       <c r="E9">
-        <v>45.264054542079997</v>
+        <v>45.26405454208</v>
       </c>
       <c r="F9">
         <v>188</v>
@@ -1178,7 +1247,7 @@
         <v>2623</v>
       </c>
       <c r="H9">
-        <v>13.952127659574471</v>
+        <v>13.95212765957447</v>
       </c>
       <c r="I9">
         <v>15</v>
@@ -1214,9 +1283,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="B10">
         <v>2019</v>
@@ -1237,7 +1306,7 @@
         <v>1228</v>
       </c>
       <c r="H10">
-        <v>18.328358208955219</v>
+        <v>18.32835820895522</v>
       </c>
       <c r="I10">
         <v>14</v>
@@ -1285,9 +1354,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="B11">
         <v>2019</v>
@@ -1308,7 +1377,7 @@
         <v>1605</v>
       </c>
       <c r="H11">
-        <v>20.316455696202532</v>
+        <v>20.31645569620253</v>
       </c>
       <c r="I11">
         <v>11</v>
@@ -1317,7 +1386,7 @@
         <v>29</v>
       </c>
       <c r="K11">
-        <v>4.3899999999999997</v>
+        <v>4.39</v>
       </c>
       <c r="L11">
         <v>40.5</v>
@@ -1332,7 +1401,7 @@
         <v>7</v>
       </c>
       <c r="P11">
-        <v>4.1500000000000004</v>
+        <v>4.15</v>
       </c>
       <c r="Q11">
         <v>171</v>
@@ -1356,9 +1425,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B12">
         <v>2020</v>
@@ -1370,7 +1439,7 @@
         <v>180.34</v>
       </c>
       <c r="E12">
-        <v>35.594006526271997</v>
+        <v>35.594006526272</v>
       </c>
       <c r="F12">
         <v>154</v>
@@ -1421,9 +1490,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="B13">
         <v>2019</v>
@@ -1435,7 +1504,7 @@
         <v>182.88</v>
       </c>
       <c r="E13">
-        <v>97.522279999999995</v>
+        <v>97.52227999999999</v>
       </c>
       <c r="F13">
         <v>148</v>
@@ -1453,7 +1522,7 @@
         <v>30</v>
       </c>
       <c r="K13">
-        <v>4.4800000000000004</v>
+        <v>4.48</v>
       </c>
       <c r="L13">
         <v>39</v>
@@ -1468,7 +1537,7 @@
         <v>7.03</v>
       </c>
       <c r="P13">
-        <v>4.1399999999999997</v>
+        <v>4.14</v>
       </c>
       <c r="Q13">
         <v>36</v>
@@ -1492,9 +1561,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2020</v>
@@ -1506,7 +1575,7 @@
         <v>190.5</v>
       </c>
       <c r="E14">
-        <v>42.589360410048002</v>
+        <v>42.589360410048</v>
       </c>
       <c r="F14">
         <v>186</v>
@@ -1563,9 +1632,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2020</v>
@@ -1577,7 +1646,7 @@
         <v>180.34</v>
       </c>
       <c r="E15">
-        <v>41.560631897728001</v>
+        <v>41.560631897728</v>
       </c>
       <c r="F15">
         <v>176</v>
@@ -1595,7 +1664,7 @@
         <v>45</v>
       </c>
       <c r="K15">
-        <v>4.3899999999999997</v>
+        <v>4.39</v>
       </c>
       <c r="L15">
         <v>35.5</v>
@@ -1631,9 +1700,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B16">
         <v>2020</v>
@@ -1645,7 +1714,7 @@
         <v>193.04</v>
       </c>
       <c r="E16">
-        <v>46.292783054399997</v>
+        <v>46.2927830544</v>
       </c>
       <c r="F16">
         <v>156</v>
@@ -1663,7 +1732,7 @@
         <v>36</v>
       </c>
       <c r="K16">
-        <v>4.4800000000000004</v>
+        <v>4.48</v>
       </c>
       <c r="L16">
         <v>36</v>
@@ -1702,9 +1771,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="B17">
         <v>2019</v>
@@ -1716,7 +1785,7 @@
         <v>177.8</v>
       </c>
       <c r="E17">
-        <v>83.007335999999995</v>
+        <v>83.007336</v>
       </c>
       <c r="F17">
         <v>135</v>
@@ -1725,7 +1794,7 @@
         <v>2235</v>
       </c>
       <c r="H17">
-        <v>16.555555555555561</v>
+        <v>16.55555555555556</v>
       </c>
       <c r="I17">
         <v>23</v>
@@ -1755,7 +1824,7 @@
         <v>66</v>
       </c>
       <c r="R17">
-        <v>69.599999999999994</v>
+        <v>69.59999999999999</v>
       </c>
       <c r="S17">
         <v>7</v>
@@ -1773,9 +1842,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B18">
         <v>2020</v>
@@ -1787,7 +1856,7 @@
         <v>187.96</v>
       </c>
       <c r="E18">
-        <v>41.972123302656001</v>
+        <v>41.972123302656</v>
       </c>
       <c r="F18">
         <v>103</v>
@@ -1805,7 +1874,7 @@
         <v>47</v>
       </c>
       <c r="K18">
-        <v>4.4800000000000004</v>
+        <v>4.48</v>
       </c>
       <c r="L18">
         <v>44.5</v>
@@ -1817,7 +1886,7 @@
         <v>187</v>
       </c>
       <c r="R18">
-        <v>64.900000000000006</v>
+        <v>64.90000000000001</v>
       </c>
       <c r="S18">
         <v>5.333333333333333</v>
@@ -1835,9 +1904,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B19">
         <v>2020</v>
@@ -1849,7 +1918,7 @@
         <v>182.88</v>
       </c>
       <c r="E19">
-        <v>40.943394790336001</v>
+        <v>40.943394790336</v>
       </c>
       <c r="F19">
         <v>68</v>
@@ -1858,7 +1927,7 @@
         <v>996</v>
       </c>
       <c r="H19">
-        <v>14.647058823529409</v>
+        <v>14.64705882352941</v>
       </c>
       <c r="I19">
         <v>15</v>
@@ -1906,9 +1975,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B20">
         <v>2020</v>
@@ -1920,7 +1989,7 @@
         <v>190.5</v>
       </c>
       <c r="E20">
-        <v>43.618088922368003</v>
+        <v>43.618088922368</v>
       </c>
       <c r="F20">
         <v>157</v>
@@ -1929,7 +1998,7 @@
         <v>2447</v>
       </c>
       <c r="H20">
-        <v>15.585987261146499</v>
+        <v>15.5859872611465</v>
       </c>
       <c r="I20">
         <v>23</v>
@@ -1977,9 +2046,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="B21">
         <v>2019</v>
@@ -1991,7 +2060,7 @@
         <v>185.42</v>
       </c>
       <c r="E21">
-        <v>97.975871999999995</v>
+        <v>97.975872</v>
       </c>
       <c r="F21">
         <v>168</v>
@@ -2024,7 +2093,7 @@
         <v>7.32</v>
       </c>
       <c r="P21">
-        <v>4.1500000000000004</v>
+        <v>4.15</v>
       </c>
       <c r="Q21">
         <v>120</v>
@@ -2048,9 +2117,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="B22">
         <v>2019</v>
@@ -2071,7 +2140,7 @@
         <v>2149</v>
       </c>
       <c r="H22">
-        <v>19.536363636363639</v>
+        <v>19.53636363636364</v>
       </c>
       <c r="I22">
         <v>18</v>
@@ -2080,7 +2149,7 @@
         <v>34</v>
       </c>
       <c r="K22">
-        <v>4.4800000000000004</v>
+        <v>4.48</v>
       </c>
       <c r="L22">
         <v>36</v>
@@ -2113,9 +2182,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B23">
         <v>2020</v>
@@ -2127,7 +2196,7 @@
         <v>182.88</v>
       </c>
       <c r="E23">
-        <v>39.091683468159999</v>
+        <v>39.09168346816</v>
       </c>
       <c r="F23">
         <v>98</v>
@@ -2136,7 +2205,7 @@
         <v>1716</v>
       </c>
       <c r="H23">
-        <v>17.510204081632651</v>
+        <v>17.51020408163265</v>
       </c>
       <c r="I23">
         <v>24</v>
@@ -2145,7 +2214,7 @@
         <v>40</v>
       </c>
       <c r="K23">
-        <v>4.2699999999999996</v>
+        <v>4.27</v>
       </c>
       <c r="L23">
         <v>42</v>
@@ -2157,7 +2226,7 @@
         <v>12</v>
       </c>
       <c r="R23">
-        <v>73.400000000000006</v>
+        <v>73.40000000000001</v>
       </c>
       <c r="S23">
         <v>2.666666666666667</v>
@@ -2175,9 +2244,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B24">
         <v>2019</v>
@@ -2189,7 +2258,7 @@
         <v>177.8</v>
       </c>
       <c r="E24">
-        <v>83.914519999999996</v>
+        <v>83.91452</v>
       </c>
       <c r="F24">
         <v>186</v>
@@ -2222,13 +2291,13 @@
         <v>6.8</v>
       </c>
       <c r="P24">
-        <v>4.1900000000000004</v>
+        <v>4.19</v>
       </c>
       <c r="Q24">
         <v>149</v>
       </c>
       <c r="R24">
-        <v>65.599999999999994</v>
+        <v>65.59999999999999</v>
       </c>
       <c r="S24">
         <v>5</v>
@@ -2246,9 +2315,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B25">
         <v>2020</v>
@@ -2260,7 +2329,7 @@
         <v>193.04</v>
       </c>
       <c r="E25">
-        <v>43.000851814976002</v>
+        <v>43.000851814976</v>
       </c>
       <c r="F25">
         <v>176</v>
@@ -2278,7 +2347,7 @@
         <v>34</v>
       </c>
       <c r="K25">
-        <v>4.6100000000000003</v>
+        <v>4.61</v>
       </c>
       <c r="L25">
         <v>36.5</v>
@@ -2299,7 +2368,7 @@
         <v>207</v>
       </c>
       <c r="R25">
-        <v>76.599999999999994</v>
+        <v>76.59999999999999</v>
       </c>
       <c r="S25">
         <v>1</v>
@@ -2317,9 +2386,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B26">
         <v>2020</v>
@@ -2340,7 +2409,7 @@
         <v>2248</v>
       </c>
       <c r="H26">
-        <v>15.189189189189189</v>
+        <v>15.18918918918919</v>
       </c>
       <c r="I26">
         <v>22</v>
@@ -2388,9 +2457,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B27">
         <v>2020</v>
@@ -2402,7 +2471,7 @@
         <v>180.34</v>
       </c>
       <c r="E27">
-        <v>39.091683468159999</v>
+        <v>39.09168346816</v>
       </c>
       <c r="F27">
         <v>301</v>
@@ -2432,7 +2501,7 @@
         <v>7.27</v>
       </c>
       <c r="P27">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="Q27">
         <v>201</v>
@@ -2456,9 +2525,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B28">
         <v>2020</v>
@@ -2470,7 +2539,7 @@
         <v>190.5</v>
       </c>
       <c r="E28">
-        <v>43.618088922368003</v>
+        <v>43.618088922368</v>
       </c>
       <c r="F28">
         <v>146</v>
@@ -2518,9 +2587,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B29">
         <v>2020</v>
@@ -2541,7 +2610,7 @@
         <v>2742</v>
       </c>
       <c r="H29">
-        <v>17.245283018867919</v>
+        <v>17.24528301886792</v>
       </c>
       <c r="I29">
         <v>26</v>
@@ -2565,7 +2634,7 @@
         <v>15</v>
       </c>
       <c r="R29">
-        <v>78.400000000000006</v>
+        <v>78.40000000000001</v>
       </c>
       <c r="S29">
         <v>5.333333333333333</v>
@@ -2583,9 +2652,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="B30">
         <v>2019</v>
@@ -2639,9 +2708,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B31">
         <v>2020</v>
@@ -2653,7 +2722,7 @@
         <v>185.42</v>
       </c>
       <c r="E31">
-        <v>44.235326029760003</v>
+        <v>44.23532602976</v>
       </c>
       <c r="F31">
         <v>129</v>
@@ -2662,7 +2731,7 @@
         <v>1465</v>
       </c>
       <c r="H31">
-        <v>11.356589147286821</v>
+        <v>11.35658914728682</v>
       </c>
       <c r="I31">
         <v>16</v>
@@ -2704,9 +2773,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B32">
         <v>2020</v>
@@ -2718,7 +2787,7 @@
         <v>187.96</v>
       </c>
       <c r="E32">
-        <v>37.651463550911998</v>
+        <v>37.651463550912</v>
       </c>
       <c r="F32">
         <v>82</v>
@@ -2727,7 +2796,7 @@
         <v>1447</v>
       </c>
       <c r="H32">
-        <v>17.646341463414629</v>
+        <v>17.64634146341463</v>
       </c>
       <c r="I32">
         <v>14</v>
@@ -2757,7 +2826,7 @@
         <v>50.5</v>
       </c>
       <c r="S32">
-        <v>0.33333333333333331</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="T32">
         <v>1</v>
@@ -2772,9 +2841,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B33">
         <v>2019</v>
@@ -2786,7 +2855,7 @@
         <v>175.26</v>
       </c>
       <c r="E33">
-        <v>82.553743999999995</v>
+        <v>82.55374399999999</v>
       </c>
       <c r="F33">
         <v>189</v>
@@ -2795,7 +2864,7 @@
         <v>2662</v>
       </c>
       <c r="H33">
-        <v>14.084656084656091</v>
+        <v>14.08465608465609</v>
       </c>
       <c r="I33">
         <v>24</v>
@@ -2804,7 +2873,7 @@
         <v>33</v>
       </c>
       <c r="K33">
-        <v>4.5599999999999996</v>
+        <v>4.56</v>
       </c>
       <c r="L33">
         <v>37</v>
@@ -2843,9 +2912,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B34">
         <v>2020</v>
@@ -2887,7 +2956,7 @@
         <v>22</v>
       </c>
       <c r="R34">
-        <v>90.4</v>
+        <v>90.40000000000001</v>
       </c>
       <c r="S34">
         <v>13</v>
@@ -2905,9 +2974,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23">
       <c r="A35" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B35">
         <v>2019</v>
@@ -2919,7 +2988,7 @@
         <v>185.42</v>
       </c>
       <c r="E35">
-        <v>95.254319999999993</v>
+        <v>95.25431999999999</v>
       </c>
       <c r="F35">
         <v>60</v>
@@ -2937,7 +3006,7 @@
         <v>21</v>
       </c>
       <c r="K35">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="Q35">
         <v>187</v>
@@ -2961,9 +3030,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B36">
         <v>2020</v>
@@ -2975,7 +3044,7 @@
         <v>182.88</v>
       </c>
       <c r="E36">
-        <v>40.737649087872001</v>
+        <v>40.737649087872</v>
       </c>
       <c r="F36">
         <v>201</v>
@@ -2993,7 +3062,7 @@
         <v>50</v>
       </c>
       <c r="K36">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="L36">
         <v>32.5</v>
@@ -3011,7 +3080,7 @@
         <v>67</v>
       </c>
       <c r="S36">
-        <v>0.33333333333333331</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="T36">
         <v>1</v>
@@ -3026,9 +3095,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B37">
         <v>2020</v>
@@ -3040,7 +3109,7 @@
         <v>180.34</v>
       </c>
       <c r="E37">
-        <v>41.766377600192001</v>
+        <v>41.766377600192</v>
       </c>
       <c r="F37">
         <v>146</v>
@@ -3049,7 +3118,7 @@
         <v>2037</v>
       </c>
       <c r="H37">
-        <v>13.952054794520549</v>
+        <v>13.95205479452055</v>
       </c>
       <c r="I37">
         <v>17</v>
@@ -3058,7 +3127,7 @@
         <v>46</v>
       </c>
       <c r="K37">
-        <v>4.4800000000000004</v>
+        <v>4.48</v>
       </c>
       <c r="L37">
         <v>37.5</v>
@@ -3073,13 +3142,13 @@
         <v>7</v>
       </c>
       <c r="P37">
-        <v>4.3499999999999996</v>
+        <v>4.35</v>
       </c>
       <c r="Q37">
         <v>176</v>
       </c>
       <c r="R37">
-        <v>65.099999999999994</v>
+        <v>65.09999999999999</v>
       </c>
       <c r="S37">
         <v>3.333333333333333</v>
@@ -3097,9 +3166,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B38">
         <v>2019</v>
@@ -3111,7 +3180,7 @@
         <v>185.42</v>
       </c>
       <c r="E38">
-        <v>91.171992000000003</v>
+        <v>91.171992</v>
       </c>
       <c r="F38">
         <v>275</v>
@@ -3129,7 +3198,7 @@
         <v>51</v>
       </c>
       <c r="K38">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="L38">
         <v>30</v>
@@ -3144,7 +3213,7 @@
         <v>7.28</v>
       </c>
       <c r="P38">
-        <v>4.2300000000000004</v>
+        <v>4.23</v>
       </c>
       <c r="Q38">
         <v>174</v>
@@ -3168,7 +3237,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23">
       <c r="A39" t="s">
         <v>59</v>
       </c>
@@ -3200,7 +3269,7 @@
         <v>35</v>
       </c>
       <c r="K39">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="L39">
         <v>32.5</v>
@@ -3239,9 +3308,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B40">
         <v>2020</v>
@@ -3253,7 +3322,7 @@
         <v>175.26</v>
       </c>
       <c r="E40">
-        <v>35.594006526271997</v>
+        <v>35.594006526272</v>
       </c>
       <c r="F40">
         <v>98</v>
@@ -3271,7 +3340,7 @@
         <v>26</v>
       </c>
       <c r="K40">
-        <v>4.2699999999999996</v>
+        <v>4.27</v>
       </c>
       <c r="M40">
         <v>15</v>
@@ -3298,9 +3367,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="B41">
         <v>2020</v>
@@ -3312,7 +3381,7 @@
         <v>187.96</v>
       </c>
       <c r="E41">
-        <v>45.264054542079997</v>
+        <v>45.26405454208</v>
       </c>
       <c r="F41">
         <v>149</v>
@@ -3357,9 +3426,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B42">
         <v>2020</v>
@@ -3371,7 +3440,7 @@
         <v>180.34</v>
       </c>
       <c r="E42">
-        <v>40.943394790336001</v>
+        <v>40.943394790336</v>
       </c>
       <c r="F42">
         <v>114</v>
@@ -3401,7 +3470,7 @@
         <v>68.8</v>
       </c>
       <c r="S42">
-        <v>0.66666666666666663</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="T42">
         <v>2</v>
@@ -3416,9 +3485,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:23">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B43">
         <v>2019</v>
@@ -3430,7 +3499,7 @@
         <v>175.26</v>
       </c>
       <c r="E43">
-        <v>77.110640000000004</v>
+        <v>77.11064</v>
       </c>
       <c r="F43">
         <v>132</v>
@@ -3439,7 +3508,7 @@
         <v>2413</v>
       </c>
       <c r="H43">
-        <v>18.280303030303031</v>
+        <v>18.28030303030303</v>
       </c>
       <c r="I43">
         <v>17</v>
@@ -3472,9 +3541,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:23">
       <c r="A44" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B44">
         <v>2019</v>
@@ -3486,7 +3555,7 @@
         <v>177.8</v>
       </c>
       <c r="E44">
-        <v>84.821703999999997</v>
+        <v>84.821704</v>
       </c>
       <c r="F44">
         <v>60</v>
@@ -3495,7 +3564,7 @@
         <v>961</v>
       </c>
       <c r="H44">
-        <v>16.016666666666669</v>
+        <v>16.01666666666667</v>
       </c>
       <c r="I44">
         <v>11</v>
@@ -3519,7 +3588,7 @@
         <v>56</v>
       </c>
       <c r="R44">
-        <v>67.900000000000006</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="S44">
         <v>5.5</v>
@@ -3537,9 +3606,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:23">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="B45">
         <v>2020</v>
@@ -3551,7 +3620,7 @@
         <v>193.04</v>
       </c>
       <c r="E45">
-        <v>45.264054542079997</v>
+        <v>45.26405454208</v>
       </c>
       <c r="F45">
         <v>171</v>
@@ -3569,7 +3638,7 @@
         <v>41</v>
       </c>
       <c r="K45">
-        <v>4.5199999999999996</v>
+        <v>4.52</v>
       </c>
       <c r="L45">
         <v>36.5</v>
@@ -3584,13 +3653,13 @@
         <v>6.96</v>
       </c>
       <c r="P45">
-        <v>4.1399999999999997</v>
+        <v>4.14</v>
       </c>
       <c r="Q45">
         <v>34</v>
       </c>
       <c r="R45">
-        <v>70.599999999999994</v>
+        <v>70.59999999999999</v>
       </c>
       <c r="S45">
         <v>7.666666666666667</v>
@@ -3608,9 +3677,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:23">
       <c r="A46" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B46">
         <v>2019</v>
@@ -3622,7 +3691,7 @@
         <v>193.04</v>
       </c>
       <c r="E46">
-        <v>99.790239999999997</v>
+        <v>99.79024</v>
       </c>
       <c r="F46">
         <v>77</v>
@@ -3631,7 +3700,7 @@
         <v>1206</v>
       </c>
       <c r="H46">
-        <v>15.662337662337659</v>
+        <v>15.66233766233766</v>
       </c>
       <c r="I46">
         <v>11</v>
@@ -3679,9 +3748,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:23">
       <c r="A47" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B47">
         <v>2019</v>
@@ -3726,7 +3795,7 @@
         <v>32</v>
       </c>
       <c r="R47">
-        <v>65.099999999999994</v>
+        <v>65.09999999999999</v>
       </c>
       <c r="S47">
         <v>1.75</v>
@@ -3744,9 +3813,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:23">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="B48">
         <v>2019</v>
@@ -3758,7 +3827,7 @@
         <v>182.88</v>
       </c>
       <c r="E48">
-        <v>92.532768000000004</v>
+        <v>92.532768</v>
       </c>
       <c r="F48">
         <v>125</v>
@@ -3767,7 +3836,7 @@
         <v>2019</v>
       </c>
       <c r="H48">
-        <v>16.152000000000001</v>
+        <v>16.152</v>
       </c>
       <c r="I48">
         <v>11</v>
@@ -3815,9 +3884,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:23">
       <c r="A49" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B49">
         <v>2019</v>
@@ -3829,7 +3898,7 @@
         <v>182.88</v>
       </c>
       <c r="E49">
-        <v>94.347136000000006</v>
+        <v>94.34713600000001</v>
       </c>
       <c r="F49">
         <v>143</v>
@@ -3847,7 +3916,7 @@
         <v>43</v>
       </c>
       <c r="K49">
-        <v>4.3099999999999996</v>
+        <v>4.31</v>
       </c>
       <c r="L49">
         <v>40</v>
@@ -3883,9 +3952,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:23">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B50">
         <v>2020</v>
@@ -3906,7 +3975,7 @@
         <v>2404</v>
       </c>
       <c r="H50">
-        <v>15.119496855345909</v>
+        <v>15.11949685534591</v>
       </c>
       <c r="I50">
         <v>17</v>
@@ -3915,7 +3984,7 @@
         <v>34</v>
       </c>
       <c r="K50">
-        <v>4.3499999999999996</v>
+        <v>4.35</v>
       </c>
       <c r="L50">
         <v>36.5</v>
@@ -3927,7 +3996,7 @@
         <v>7.28</v>
       </c>
       <c r="P50">
-        <v>4.3600000000000003</v>
+        <v>4.36</v>
       </c>
       <c r="Q50">
         <v>200</v>
@@ -3951,9 +4020,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:23">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="B51">
         <v>2020</v>
@@ -3965,7 +4034,7 @@
         <v>185.42</v>
       </c>
       <c r="E51">
-        <v>42.795106112512002</v>
+        <v>42.795106112512</v>
       </c>
       <c r="F51">
         <v>93</v>
@@ -3983,7 +4052,7 @@
         <v>30</v>
       </c>
       <c r="K51">
-        <v>4.7300000000000004</v>
+        <v>4.73</v>
       </c>
       <c r="L51">
         <v>38.5</v>
@@ -4022,9 +4091,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:23">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B52">
         <v>2019</v>
@@ -4036,7 +4105,7 @@
         <v>185.42</v>
       </c>
       <c r="E52">
-        <v>90.264808000000002</v>
+        <v>90.264808</v>
       </c>
       <c r="F52">
         <v>69</v>
@@ -4045,7 +4114,7 @@
         <v>1015</v>
       </c>
       <c r="H52">
-        <v>14.710144927536231</v>
+        <v>14.71014492753623</v>
       </c>
       <c r="I52">
         <v>13</v>
@@ -4093,9 +4162,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:23">
       <c r="A53" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="B53">
         <v>2019</v>
@@ -4107,7 +4176,7 @@
         <v>175.26</v>
       </c>
       <c r="E53">
-        <v>78.925008000000005</v>
+        <v>78.92500800000001</v>
       </c>
       <c r="F53">
         <v>215</v>
@@ -4116,7 +4185,7 @@
         <v>2867</v>
       </c>
       <c r="H53">
-        <v>13.334883720930231</v>
+        <v>13.33488372093023</v>
       </c>
       <c r="I53">
         <v>23</v>
@@ -4125,7 +4194,7 @@
         <v>45</v>
       </c>
       <c r="K53">
-        <v>4.3600000000000003</v>
+        <v>4.36</v>
       </c>
       <c r="L53">
         <v>34</v>
@@ -4140,7 +4209,7 @@
         <v>6.97</v>
       </c>
       <c r="P53">
-        <v>4.0199999999999996</v>
+        <v>4.02</v>
       </c>
       <c r="Q53">
         <v>208</v>
@@ -4164,9 +4233,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:23">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B54">
         <v>2020</v>
@@ -4178,7 +4247,7 @@
         <v>193.04</v>
       </c>
       <c r="E54">
-        <v>45.058308839615997</v>
+        <v>45.058308839616</v>
       </c>
       <c r="F54">
         <v>135</v>
@@ -4187,7 +4256,7 @@
         <v>2448</v>
       </c>
       <c r="H54">
-        <v>18.133333333333329</v>
+        <v>18.13333333333333</v>
       </c>
       <c r="I54">
         <v>27</v>
@@ -4202,10 +4271,10 @@
         <v>33</v>
       </c>
       <c r="R54">
-        <v>77.099999999999994</v>
+        <v>77.09999999999999</v>
       </c>
       <c r="S54">
-        <v>8.6666666666666661</v>
+        <v>8.666666666666666</v>
       </c>
       <c r="T54">
         <v>26</v>
@@ -4220,9 +4289,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:23">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="B55">
         <v>2019</v>
@@ -4234,7 +4303,7 @@
         <v>180.34</v>
       </c>
       <c r="E55">
-        <v>83.914519999999996</v>
+        <v>83.91452</v>
       </c>
       <c r="F55">
         <v>134</v>
@@ -4243,7 +4312,7 @@
         <v>1800</v>
       </c>
       <c r="H55">
-        <v>13.432835820895519</v>
+        <v>13.43283582089552</v>
       </c>
       <c r="I55">
         <v>11</v>
@@ -4285,9 +4354,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:23">
       <c r="A56" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B56">
         <v>2019</v>
@@ -4299,7 +4368,7 @@
         <v>182.88</v>
       </c>
       <c r="E56">
-        <v>95.254319999999993</v>
+        <v>95.25431999999999</v>
       </c>
       <c r="F56">
         <v>75</v>
@@ -4317,7 +4386,7 @@
         <v>44</v>
       </c>
       <c r="K56">
-        <v>4.3499999999999996</v>
+        <v>4.35</v>
       </c>
       <c r="L56">
         <v>37.5</v>
@@ -4332,13 +4401,13 @@
         <v>7.01</v>
       </c>
       <c r="P56">
-        <v>4.1500000000000004</v>
+        <v>4.15</v>
       </c>
       <c r="Q56">
         <v>76</v>
       </c>
       <c r="R56">
-        <v>79.900000000000006</v>
+        <v>79.90000000000001</v>
       </c>
       <c r="S56">
         <v>7.75</v>
@@ -4356,9 +4425,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:23">
       <c r="A57" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B57">
         <v>2019</v>
@@ -4370,7 +4439,7 @@
         <v>190.5</v>
       </c>
       <c r="E57">
-        <v>97.522279999999995</v>
+        <v>97.52227999999999</v>
       </c>
       <c r="F57">
         <v>128</v>
@@ -4421,9 +4490,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:23">
       <c r="A58" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="B58">
         <v>2020</v>
@@ -4435,7 +4504,7 @@
         <v>185.42</v>
       </c>
       <c r="E58">
-        <v>42.383614707584002</v>
+        <v>42.383614707584</v>
       </c>
       <c r="F58">
         <v>213</v>
@@ -4477,9 +4546,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:23">
       <c r="A59" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="B59">
         <v>2020</v>
@@ -4491,7 +4560,7 @@
         <v>185.42</v>
       </c>
       <c r="E59">
-        <v>41.149140492800001</v>
+        <v>41.1491404928</v>
       </c>
       <c r="F59">
         <v>175</v>
@@ -4509,13 +4578,13 @@
         <v>45</v>
       </c>
       <c r="K59">
-        <v>4.3899999999999997</v>
+        <v>4.39</v>
       </c>
       <c r="Q59">
         <v>57</v>
       </c>
       <c r="R59">
-        <v>68.400000000000006</v>
+        <v>68.40000000000001</v>
       </c>
       <c r="S59">
         <v>4.333333333333333</v>
@@ -4533,10 +4602,1805 @@
         <v>3</v>
       </c>
     </row>
+    <row r="60" spans="1:23">
+      <c r="A60" t="s">
+        <v>80</v>
+      </c>
+      <c r="B60">
+        <v>2018</v>
+      </c>
+      <c r="C60">
+        <v>23</v>
+      </c>
+      <c r="D60">
+        <v>190.5</v>
+      </c>
+      <c r="E60">
+        <v>93.89354400000001</v>
+      </c>
+      <c r="F60">
+        <v>158</v>
+      </c>
+      <c r="G60">
+        <v>2477</v>
+      </c>
+      <c r="H60">
+        <v>15.67721518987342</v>
+      </c>
+      <c r="I60">
+        <v>21</v>
+      </c>
+      <c r="J60">
+        <v>47</v>
+      </c>
+      <c r="K60">
+        <v>4.6</v>
+      </c>
+      <c r="L60">
+        <v>38</v>
+      </c>
+      <c r="M60">
+        <v>21</v>
+      </c>
+      <c r="N60">
+        <v>120</v>
+      </c>
+      <c r="O60">
+        <v>6.56</v>
+      </c>
+      <c r="P60">
+        <v>4.04</v>
+      </c>
+      <c r="Q60">
+        <v>265</v>
+      </c>
+      <c r="R60">
+        <v>53.5</v>
+      </c>
+      <c r="S60">
+        <v>0</v>
+      </c>
+      <c r="T60">
+        <v>0</v>
+      </c>
+      <c r="W60">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23">
+      <c r="A61" t="s">
+        <v>81</v>
+      </c>
+      <c r="B61">
+        <v>2018</v>
+      </c>
+      <c r="C61">
+        <v>23</v>
+      </c>
+      <c r="D61">
+        <v>195.58</v>
+      </c>
+      <c r="E61">
+        <v>98.883056</v>
+      </c>
+      <c r="F61">
+        <v>99</v>
+      </c>
+      <c r="G61">
+        <v>1362</v>
+      </c>
+      <c r="H61">
+        <v>13.75757575757576</v>
+      </c>
+      <c r="I61">
+        <v>14</v>
+      </c>
+      <c r="J61">
+        <v>23</v>
+      </c>
+      <c r="K61">
+        <v>4.56</v>
+      </c>
+      <c r="L61">
+        <v>34.5</v>
+      </c>
+      <c r="M61">
+        <v>16</v>
+      </c>
+      <c r="N61">
+        <v>124</v>
+      </c>
+      <c r="O61">
+        <v>7.2</v>
+      </c>
+      <c r="P61">
+        <v>4.4</v>
+      </c>
+      <c r="Q61">
+        <v>132</v>
+      </c>
+      <c r="R61">
+        <v>78.3</v>
+      </c>
+      <c r="S61">
+        <v>0</v>
+      </c>
+      <c r="T61">
+        <v>0</v>
+      </c>
+      <c r="W61">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23">
+      <c r="A62" t="s">
+        <v>82</v>
+      </c>
+      <c r="B62">
+        <v>2018</v>
+      </c>
+      <c r="C62">
+        <v>23</v>
+      </c>
+      <c r="D62">
+        <v>185.42</v>
+      </c>
+      <c r="E62">
+        <v>90.264808</v>
+      </c>
+      <c r="F62">
+        <v>214</v>
+      </c>
+      <c r="G62">
+        <v>2842</v>
+      </c>
+      <c r="H62">
+        <v>13.2803738317757</v>
+      </c>
+      <c r="I62">
+        <v>18</v>
+      </c>
+      <c r="J62">
+        <v>50</v>
+      </c>
+      <c r="L62">
+        <v>34.5</v>
+      </c>
+      <c r="N62">
+        <v>118</v>
+      </c>
+      <c r="O62">
+        <v>6.84</v>
+      </c>
+      <c r="P62">
+        <v>4.15</v>
+      </c>
+      <c r="Q62">
+        <v>113</v>
+      </c>
+      <c r="R62">
+        <v>58.4</v>
+      </c>
+      <c r="S62">
+        <v>1.2</v>
+      </c>
+      <c r="T62">
+        <v>6</v>
+      </c>
+      <c r="W62">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23">
+      <c r="A63" t="s">
+        <v>83</v>
+      </c>
+      <c r="B63">
+        <v>2018</v>
+      </c>
+      <c r="C63">
+        <v>21</v>
+      </c>
+      <c r="D63">
+        <v>180.34</v>
+      </c>
+      <c r="E63">
+        <v>90.7184</v>
+      </c>
+      <c r="F63">
+        <v>89</v>
+      </c>
+      <c r="G63">
+        <v>1399</v>
+      </c>
+      <c r="H63">
+        <v>15.71910112359551</v>
+      </c>
+      <c r="I63">
+        <v>7</v>
+      </c>
+      <c r="J63">
+        <v>26</v>
+      </c>
+      <c r="K63">
+        <v>4.41</v>
+      </c>
+      <c r="L63">
+        <v>43</v>
+      </c>
+      <c r="N63">
+        <v>121</v>
+      </c>
+      <c r="Q63">
+        <v>105</v>
+      </c>
+      <c r="R63">
+        <v>60.5</v>
+      </c>
+      <c r="S63">
+        <v>1</v>
+      </c>
+      <c r="T63">
+        <v>5</v>
+      </c>
+      <c r="W63">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23">
+      <c r="A64" t="s">
+        <v>84</v>
+      </c>
+      <c r="B64">
+        <v>2018</v>
+      </c>
+      <c r="C64">
+        <v>21</v>
+      </c>
+      <c r="D64">
+        <v>177.8</v>
+      </c>
+      <c r="E64">
+        <v>82.10015199999999</v>
+      </c>
+      <c r="F64">
+        <v>159</v>
+      </c>
+      <c r="G64">
+        <v>2424</v>
+      </c>
+      <c r="H64">
+        <v>15.24528301886792</v>
+      </c>
+      <c r="I64">
+        <v>17</v>
+      </c>
+      <c r="J64">
+        <v>30</v>
+      </c>
+      <c r="K64">
+        <v>4.43</v>
+      </c>
+      <c r="L64">
+        <v>34.5</v>
+      </c>
+      <c r="M64">
+        <v>14</v>
+      </c>
+      <c r="N64">
+        <v>113</v>
+      </c>
+      <c r="O64">
+        <v>6.93</v>
+      </c>
+      <c r="P64">
+        <v>4.15</v>
+      </c>
+      <c r="Q64">
+        <v>103</v>
+      </c>
+      <c r="R64">
+        <v>37.5</v>
+      </c>
+      <c r="S64">
+        <v>1.4</v>
+      </c>
+      <c r="T64">
+        <v>7</v>
+      </c>
+      <c r="W64">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23">
+      <c r="A65" t="s">
+        <v>85</v>
+      </c>
+      <c r="B65">
+        <v>2018</v>
+      </c>
+      <c r="C65">
+        <v>22</v>
+      </c>
+      <c r="D65">
+        <v>187.96</v>
+      </c>
+      <c r="E65">
+        <v>92.079176</v>
+      </c>
+      <c r="F65">
+        <v>168</v>
+      </c>
+      <c r="G65">
+        <v>2748</v>
+      </c>
+      <c r="H65">
+        <v>16.35714285714286</v>
+      </c>
+      <c r="I65">
+        <v>22</v>
+      </c>
+      <c r="J65">
+        <v>37</v>
+      </c>
+      <c r="K65">
+        <v>4.49</v>
+      </c>
+      <c r="L65">
+        <v>37.5</v>
+      </c>
+      <c r="M65">
+        <v>12</v>
+      </c>
+      <c r="N65">
+        <v>130</v>
+      </c>
+      <c r="O65">
+        <v>6.97</v>
+      </c>
+      <c r="P65">
+        <v>4.5</v>
+      </c>
+      <c r="Q65">
+        <v>265</v>
+      </c>
+      <c r="R65">
+        <v>69</v>
+      </c>
+      <c r="S65">
+        <v>3</v>
+      </c>
+      <c r="T65">
+        <v>15</v>
+      </c>
+      <c r="W65">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23">
+      <c r="A66" t="s">
+        <v>86</v>
+      </c>
+      <c r="B66">
+        <v>2018</v>
+      </c>
+      <c r="C66">
+        <v>22</v>
+      </c>
+      <c r="D66">
+        <v>185.42</v>
+      </c>
+      <c r="E66">
+        <v>92.98636</v>
+      </c>
+      <c r="F66">
+        <v>176</v>
+      </c>
+      <c r="G66">
+        <v>2690</v>
+      </c>
+      <c r="H66">
+        <v>15.28409090909091</v>
+      </c>
+      <c r="I66">
+        <v>21</v>
+      </c>
+      <c r="J66">
+        <v>26</v>
+      </c>
+      <c r="K66">
+        <v>4.51</v>
+      </c>
+      <c r="L66">
+        <v>36</v>
+      </c>
+      <c r="M66">
+        <v>10</v>
+      </c>
+      <c r="N66">
+        <v>122</v>
+      </c>
+      <c r="O66">
+        <v>6.95</v>
+      </c>
+      <c r="P66">
+        <v>4.37</v>
+      </c>
+      <c r="Q66">
+        <v>81</v>
+      </c>
+      <c r="R66">
+        <v>62.8</v>
+      </c>
+      <c r="S66">
+        <v>5.2</v>
+      </c>
+      <c r="T66">
+        <v>26</v>
+      </c>
+      <c r="W66">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23">
+      <c r="A67" t="s">
+        <v>87</v>
+      </c>
+      <c r="B67">
+        <v>2018</v>
+      </c>
+      <c r="C67">
+        <v>21</v>
+      </c>
+      <c r="D67">
+        <v>190.5</v>
+      </c>
+      <c r="E67">
+        <v>90.264808</v>
+      </c>
+      <c r="F67">
+        <v>66</v>
+      </c>
+      <c r="G67">
+        <v>1351</v>
+      </c>
+      <c r="H67">
+        <v>20.46969696969697</v>
+      </c>
+      <c r="I67">
+        <v>6</v>
+      </c>
+      <c r="J67">
+        <v>25</v>
+      </c>
+      <c r="K67">
+        <v>4.34</v>
+      </c>
+      <c r="L67">
+        <v>40</v>
+      </c>
+      <c r="M67">
+        <v>16</v>
+      </c>
+      <c r="N67">
+        <v>129</v>
+      </c>
+      <c r="Q67">
+        <v>61</v>
+      </c>
+      <c r="R67">
+        <v>69.59999999999999</v>
+      </c>
+      <c r="S67">
+        <v>3.6</v>
+      </c>
+      <c r="T67">
+        <v>18</v>
+      </c>
+      <c r="W67">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23">
+      <c r="A68" t="s">
+        <v>88</v>
+      </c>
+      <c r="B68">
+        <v>2018</v>
+      </c>
+      <c r="C68">
+        <v>22</v>
+      </c>
+      <c r="D68">
+        <v>180.34</v>
+      </c>
+      <c r="E68">
+        <v>96.61509599999999</v>
+      </c>
+      <c r="F68">
+        <v>226</v>
+      </c>
+      <c r="G68">
+        <v>4472</v>
+      </c>
+      <c r="H68">
+        <v>19.78761061946903</v>
+      </c>
+      <c r="I68">
+        <v>39</v>
+      </c>
+      <c r="J68">
+        <v>51</v>
+      </c>
+      <c r="K68">
+        <v>4.54</v>
+      </c>
+      <c r="L68">
+        <v>34.5</v>
+      </c>
+      <c r="M68">
+        <v>14</v>
+      </c>
+      <c r="N68">
+        <v>120</v>
+      </c>
+      <c r="O68">
+        <v>7.11</v>
+      </c>
+      <c r="P68">
+        <v>4.32</v>
+      </c>
+      <c r="Q68">
+        <v>60</v>
+      </c>
+      <c r="R68">
+        <v>52.3</v>
+      </c>
+      <c r="S68">
+        <v>2.2</v>
+      </c>
+      <c r="T68">
+        <v>11</v>
+      </c>
+      <c r="W68">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23">
+      <c r="A69" t="s">
+        <v>89</v>
+      </c>
+      <c r="B69">
+        <v>2018</v>
+      </c>
+      <c r="C69">
+        <v>23</v>
+      </c>
+      <c r="D69">
+        <v>180.34</v>
+      </c>
+      <c r="E69">
+        <v>91.171992</v>
+      </c>
+      <c r="F69">
+        <v>238</v>
+      </c>
+      <c r="G69">
+        <v>3590</v>
+      </c>
+      <c r="H69">
+        <v>15.08403361344538</v>
+      </c>
+      <c r="I69">
+        <v>37</v>
+      </c>
+      <c r="J69">
+        <v>38</v>
+      </c>
+      <c r="K69">
+        <v>4.5</v>
+      </c>
+      <c r="L69">
+        <v>39</v>
+      </c>
+      <c r="M69">
+        <v>22</v>
+      </c>
+      <c r="N69">
+        <v>125</v>
+      </c>
+      <c r="O69">
+        <v>6.65</v>
+      </c>
+      <c r="P69">
+        <v>4.26</v>
+      </c>
+      <c r="Q69">
+        <v>51</v>
+      </c>
+      <c r="R69">
+        <v>61.9</v>
+      </c>
+      <c r="S69">
+        <v>2.4</v>
+      </c>
+      <c r="T69">
+        <v>12</v>
+      </c>
+      <c r="W69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23">
+      <c r="A70" t="s">
+        <v>90</v>
+      </c>
+      <c r="B70">
+        <v>2018</v>
+      </c>
+      <c r="C70">
+        <v>21</v>
+      </c>
+      <c r="D70">
+        <v>177.8</v>
+      </c>
+      <c r="E70">
+        <v>91.171992</v>
+      </c>
+      <c r="F70">
+        <v>234</v>
+      </c>
+      <c r="G70">
+        <v>2856</v>
+      </c>
+      <c r="H70">
+        <v>12.2051282051282</v>
+      </c>
+      <c r="I70">
+        <v>26</v>
+      </c>
+      <c r="J70">
+        <v>39</v>
+      </c>
+      <c r="K70">
+        <v>4.47</v>
+      </c>
+      <c r="L70">
+        <v>35.5</v>
+      </c>
+      <c r="M70">
+        <v>20</v>
+      </c>
+      <c r="N70">
+        <v>115</v>
+      </c>
+      <c r="O70">
+        <v>7.09</v>
+      </c>
+      <c r="P70">
+        <v>4.45</v>
+      </c>
+      <c r="Q70">
+        <v>47</v>
+      </c>
+      <c r="R70">
+        <v>74.2</v>
+      </c>
+      <c r="S70">
+        <v>6.6</v>
+      </c>
+      <c r="T70">
+        <v>33</v>
+      </c>
+      <c r="W70">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23">
+      <c r="A71" t="s">
+        <v>91</v>
+      </c>
+      <c r="B71">
+        <v>2018</v>
+      </c>
+      <c r="C71">
+        <v>22</v>
+      </c>
+      <c r="D71">
+        <v>182.88</v>
+      </c>
+      <c r="E71">
+        <v>84.368112</v>
+      </c>
+      <c r="F71">
+        <v>163</v>
+      </c>
+      <c r="G71">
+        <v>2256</v>
+      </c>
+      <c r="H71">
+        <v>13.84049079754601</v>
+      </c>
+      <c r="I71">
+        <v>24</v>
+      </c>
+      <c r="J71">
+        <v>52</v>
+      </c>
+      <c r="Q71">
+        <v>44</v>
+      </c>
+      <c r="R71">
+        <v>68.3</v>
+      </c>
+      <c r="S71">
+        <v>1.8</v>
+      </c>
+      <c r="T71">
+        <v>9</v>
+      </c>
+      <c r="W71">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23">
+      <c r="A72" t="s">
+        <v>92</v>
+      </c>
+      <c r="B72">
+        <v>2018</v>
+      </c>
+      <c r="C72">
+        <v>22</v>
+      </c>
+      <c r="D72">
+        <v>190.5</v>
+      </c>
+      <c r="E72">
+        <v>98.883056</v>
+      </c>
+      <c r="F72">
+        <v>195</v>
+      </c>
+      <c r="G72">
+        <v>3220</v>
+      </c>
+      <c r="H72">
+        <v>16.51282051282051</v>
+      </c>
+      <c r="I72">
+        <v>31</v>
+      </c>
+      <c r="J72">
+        <v>40</v>
+      </c>
+      <c r="K72">
+        <v>4.54</v>
+      </c>
+      <c r="L72">
+        <v>35.5</v>
+      </c>
+      <c r="M72">
+        <v>18</v>
+      </c>
+      <c r="N72">
+        <v>124</v>
+      </c>
+      <c r="O72">
+        <v>6.57</v>
+      </c>
+      <c r="P72">
+        <v>4.11</v>
+      </c>
+      <c r="Q72">
+        <v>40</v>
+      </c>
+      <c r="R72">
+        <v>71.2</v>
+      </c>
+      <c r="S72">
+        <v>4.8</v>
+      </c>
+      <c r="T72">
+        <v>24</v>
+      </c>
+      <c r="W72">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23">
+      <c r="A73" t="s">
+        <v>93</v>
+      </c>
+      <c r="B73">
+        <v>2018</v>
+      </c>
+      <c r="C73">
+        <v>23</v>
+      </c>
+      <c r="D73">
+        <v>182.88</v>
+      </c>
+      <c r="E73">
+        <v>85.728888</v>
+      </c>
+      <c r="F73">
+        <v>224</v>
+      </c>
+      <c r="G73">
+        <v>2781</v>
+      </c>
+      <c r="H73">
+        <v>12.41517857142857</v>
+      </c>
+      <c r="I73">
+        <v>19</v>
+      </c>
+      <c r="J73">
+        <v>44</v>
+      </c>
+      <c r="K73">
+        <v>4.43</v>
+      </c>
+      <c r="L73">
+        <v>31</v>
+      </c>
+      <c r="M73">
+        <v>15</v>
+      </c>
+      <c r="N73">
+        <v>110</v>
+      </c>
+      <c r="O73">
+        <v>6.88</v>
+      </c>
+      <c r="P73">
+        <v>4.41</v>
+      </c>
+      <c r="Q73">
+        <v>26</v>
+      </c>
+      <c r="R73">
+        <v>64.3</v>
+      </c>
+      <c r="S73">
+        <v>5.2</v>
+      </c>
+      <c r="T73">
+        <v>26</v>
+      </c>
+      <c r="W73">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23">
+      <c r="A74" t="s">
+        <v>94</v>
+      </c>
+      <c r="B74">
+        <v>2018</v>
+      </c>
+      <c r="C74">
+        <v>21</v>
+      </c>
+      <c r="D74">
+        <v>182.88</v>
+      </c>
+      <c r="E74">
+        <v>95.25431999999999</v>
+      </c>
+      <c r="F74">
+        <v>146</v>
+      </c>
+      <c r="G74">
+        <v>2027</v>
+      </c>
+      <c r="H74">
+        <v>13.88356164383562</v>
+      </c>
+      <c r="I74">
+        <v>17</v>
+      </c>
+      <c r="J74">
+        <v>36</v>
+      </c>
+      <c r="K74">
+        <v>4.42</v>
+      </c>
+      <c r="L74">
+        <v>39.5</v>
+      </c>
+      <c r="M74">
+        <v>15</v>
+      </c>
+      <c r="N74">
+        <v>132</v>
+      </c>
+      <c r="O74">
+        <v>6.95</v>
+      </c>
+      <c r="P74">
+        <v>4.07</v>
+      </c>
+      <c r="Q74">
+        <v>24</v>
+      </c>
+      <c r="R74">
+        <v>88.3</v>
+      </c>
+      <c r="S74">
+        <v>7.8</v>
+      </c>
+      <c r="T74">
+        <v>39</v>
+      </c>
+      <c r="W74">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23">
+      <c r="A75" t="s">
+        <v>95</v>
+      </c>
+      <c r="B75">
+        <v>2018</v>
+      </c>
+      <c r="C75">
+        <v>22</v>
+      </c>
+      <c r="D75">
+        <v>180.34</v>
+      </c>
+      <c r="E75">
+        <v>92.079176</v>
+      </c>
+      <c r="F75">
+        <v>136</v>
+      </c>
+      <c r="G75">
+        <v>1512</v>
+      </c>
+      <c r="H75">
+        <v>11.11764705882353</v>
+      </c>
+      <c r="I75">
+        <v>13</v>
+      </c>
+      <c r="J75">
+        <v>27</v>
+      </c>
+      <c r="K75">
+        <v>4.55</v>
+      </c>
+      <c r="L75">
+        <v>33.5</v>
+      </c>
+      <c r="M75">
+        <v>17</v>
+      </c>
+      <c r="N75">
+        <v>116</v>
+      </c>
+      <c r="O75">
+        <v>6.91</v>
+      </c>
+      <c r="P75">
+        <v>4.19</v>
+      </c>
+      <c r="Q75">
+        <v>256</v>
+      </c>
+      <c r="R75">
+        <v>54.1</v>
+      </c>
+      <c r="S75">
+        <v>0.4</v>
+      </c>
+      <c r="T75">
+        <v>2</v>
+      </c>
+      <c r="W75">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23">
+      <c r="A76" t="s">
+        <v>96</v>
+      </c>
+      <c r="B76">
+        <v>2018</v>
+      </c>
+      <c r="C76">
+        <v>21</v>
+      </c>
+      <c r="D76">
+        <v>195.58</v>
+      </c>
+      <c r="E76">
+        <v>103.418976</v>
+      </c>
+      <c r="F76">
+        <v>65</v>
+      </c>
+      <c r="G76">
+        <v>957</v>
+      </c>
+      <c r="H76">
+        <v>14.72307692307692</v>
+      </c>
+      <c r="I76">
+        <v>16</v>
+      </c>
+      <c r="J76">
+        <v>22</v>
+      </c>
+      <c r="K76">
+        <v>4.68</v>
+      </c>
+      <c r="L76">
+        <v>31</v>
+      </c>
+      <c r="N76">
+        <v>112</v>
+      </c>
+      <c r="Q76">
+        <v>253</v>
+      </c>
+      <c r="R76">
+        <v>69.59999999999999</v>
+      </c>
+      <c r="S76">
+        <v>1</v>
+      </c>
+      <c r="T76">
+        <v>5</v>
+      </c>
+      <c r="W76">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:23">
+      <c r="A77" t="s">
+        <v>97</v>
+      </c>
+      <c r="B77">
+        <v>2018</v>
+      </c>
+      <c r="C77">
+        <v>23</v>
+      </c>
+      <c r="D77">
+        <v>177.8</v>
+      </c>
+      <c r="E77">
+        <v>83.007336</v>
+      </c>
+      <c r="F77">
+        <v>243</v>
+      </c>
+      <c r="G77">
+        <v>3249</v>
+      </c>
+      <c r="H77">
+        <v>13.37037037037037</v>
+      </c>
+      <c r="I77">
+        <v>23</v>
+      </c>
+      <c r="J77">
+        <v>31</v>
+      </c>
+      <c r="K77">
+        <v>4.48</v>
+      </c>
+      <c r="L77">
+        <v>35.5</v>
+      </c>
+      <c r="M77">
+        <v>6</v>
+      </c>
+      <c r="N77">
+        <v>122</v>
+      </c>
+      <c r="O77">
+        <v>6.87</v>
+      </c>
+      <c r="P77">
+        <v>4.16</v>
+      </c>
+      <c r="Q77">
+        <v>240</v>
+      </c>
+      <c r="R77">
+        <v>51</v>
+      </c>
+      <c r="S77">
+        <v>2.4</v>
+      </c>
+      <c r="T77">
+        <v>12</v>
+      </c>
+      <c r="W77">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:23">
+      <c r="A78" t="s">
+        <v>98</v>
+      </c>
+      <c r="B78">
+        <v>2018</v>
+      </c>
+      <c r="C78">
+        <v>23</v>
+      </c>
+      <c r="D78">
+        <v>193.04</v>
+      </c>
+      <c r="E78">
+        <v>97.975872</v>
+      </c>
+      <c r="F78">
+        <v>146</v>
+      </c>
+      <c r="G78">
+        <v>2466</v>
+      </c>
+      <c r="H78">
+        <v>16.89041095890411</v>
+      </c>
+      <c r="I78">
+        <v>13</v>
+      </c>
+      <c r="J78">
+        <v>43</v>
+      </c>
+      <c r="K78">
+        <v>4.62</v>
+      </c>
+      <c r="L78">
+        <v>34</v>
+      </c>
+      <c r="M78">
+        <v>13</v>
+      </c>
+      <c r="N78">
+        <v>121</v>
+      </c>
+      <c r="O78">
+        <v>7.07</v>
+      </c>
+      <c r="P78">
+        <v>4.25</v>
+      </c>
+      <c r="Q78">
+        <v>228</v>
+      </c>
+      <c r="R78">
+        <v>45</v>
+      </c>
+      <c r="S78">
+        <v>0.4</v>
+      </c>
+      <c r="T78">
+        <v>2</v>
+      </c>
+      <c r="W78">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:23">
+      <c r="A79" t="s">
+        <v>99</v>
+      </c>
+      <c r="B79">
+        <v>2018</v>
+      </c>
+      <c r="C79">
+        <v>23</v>
+      </c>
+      <c r="D79">
+        <v>190.5</v>
+      </c>
+      <c r="E79">
+        <v>97.52227999999999</v>
+      </c>
+      <c r="F79">
+        <v>62</v>
+      </c>
+      <c r="G79">
+        <v>910</v>
+      </c>
+      <c r="H79">
+        <v>14.67741935483871</v>
+      </c>
+      <c r="I79">
+        <v>8</v>
+      </c>
+      <c r="J79">
+        <v>22</v>
+      </c>
+      <c r="K79">
+        <v>4.53</v>
+      </c>
+      <c r="L79">
+        <v>33.5</v>
+      </c>
+      <c r="N79">
+        <v>113</v>
+      </c>
+      <c r="O79">
+        <v>7</v>
+      </c>
+      <c r="Q79">
+        <v>224</v>
+      </c>
+      <c r="R79">
+        <v>53.9</v>
+      </c>
+      <c r="S79">
+        <v>0.2</v>
+      </c>
+      <c r="T79">
+        <v>1</v>
+      </c>
+      <c r="W79">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:23">
+      <c r="A80" t="s">
+        <v>100</v>
+      </c>
+      <c r="B80">
+        <v>2018</v>
+      </c>
+      <c r="C80">
+        <v>22</v>
+      </c>
+      <c r="D80">
+        <v>175.26</v>
+      </c>
+      <c r="E80">
+        <v>83.460928</v>
+      </c>
+      <c r="F80">
+        <v>100</v>
+      </c>
+      <c r="G80">
+        <v>1175</v>
+      </c>
+      <c r="H80">
+        <v>11.75</v>
+      </c>
+      <c r="I80">
+        <v>14</v>
+      </c>
+      <c r="J80">
+        <v>46</v>
+      </c>
+      <c r="K80">
+        <v>4.44</v>
+      </c>
+      <c r="L80">
+        <v>36</v>
+      </c>
+      <c r="M80">
+        <v>11</v>
+      </c>
+      <c r="N80">
+        <v>110</v>
+      </c>
+      <c r="O80">
+        <v>6.72</v>
+      </c>
+      <c r="P80">
+        <v>4.18</v>
+      </c>
+      <c r="Q80">
+        <v>210</v>
+      </c>
+      <c r="R80">
+        <v>70.09999999999999</v>
+      </c>
+      <c r="S80">
+        <v>2</v>
+      </c>
+      <c r="T80">
+        <v>10</v>
+      </c>
+      <c r="W80">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23">
+      <c r="A81" t="s">
+        <v>101</v>
+      </c>
+      <c r="B81">
+        <v>2018</v>
+      </c>
+      <c r="C81">
+        <v>22</v>
+      </c>
+      <c r="D81">
+        <v>187.96</v>
+      </c>
+      <c r="E81">
+        <v>89.357624</v>
+      </c>
+      <c r="F81">
+        <v>139</v>
+      </c>
+      <c r="G81">
+        <v>2640</v>
+      </c>
+      <c r="H81">
+        <v>18.99280575539568</v>
+      </c>
+      <c r="I81">
+        <v>18</v>
+      </c>
+      <c r="J81">
+        <v>26</v>
+      </c>
+      <c r="K81">
+        <v>4.55</v>
+      </c>
+      <c r="L81">
+        <v>37</v>
+      </c>
+      <c r="M81">
+        <v>9</v>
+      </c>
+      <c r="N81">
+        <v>121</v>
+      </c>
+      <c r="O81">
+        <v>6.89</v>
+      </c>
+      <c r="P81">
+        <v>4.23</v>
+      </c>
+      <c r="Q81">
+        <v>208</v>
+      </c>
+      <c r="R81">
+        <v>58.1</v>
+      </c>
+      <c r="S81">
+        <v>1.4</v>
+      </c>
+      <c r="T81">
+        <v>7</v>
+      </c>
+      <c r="W81">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:23">
+      <c r="A82" t="s">
+        <v>102</v>
+      </c>
+      <c r="B82">
+        <v>2018</v>
+      </c>
+      <c r="C82">
+        <v>21</v>
+      </c>
+      <c r="D82">
+        <v>195.58</v>
+      </c>
+      <c r="E82">
+        <v>97.06868799999999</v>
+      </c>
+      <c r="F82">
+        <v>92</v>
+      </c>
+      <c r="G82">
+        <v>1484</v>
+      </c>
+      <c r="H82">
+        <v>16.1304347826087</v>
+      </c>
+      <c r="I82">
+        <v>13</v>
+      </c>
+      <c r="J82">
+        <v>26</v>
+      </c>
+      <c r="K82">
+        <v>4.48</v>
+      </c>
+      <c r="M82">
+        <v>20</v>
+      </c>
+      <c r="Q82">
+        <v>207</v>
+      </c>
+      <c r="R82">
+        <v>64.2</v>
+      </c>
+      <c r="S82">
+        <v>1.6</v>
+      </c>
+      <c r="T82">
+        <v>8</v>
+      </c>
+      <c r="W82">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:23">
+      <c r="A83" t="s">
+        <v>103</v>
+      </c>
+      <c r="B83">
+        <v>2018</v>
+      </c>
+      <c r="C83">
+        <v>22</v>
+      </c>
+      <c r="D83">
+        <v>182.88</v>
+      </c>
+      <c r="E83">
+        <v>83.460928</v>
+      </c>
+      <c r="F83">
+        <v>28</v>
+      </c>
+      <c r="G83">
+        <v>232</v>
+      </c>
+      <c r="H83">
+        <v>8.285714285714286</v>
+      </c>
+      <c r="I83">
+        <v>1</v>
+      </c>
+      <c r="J83">
+        <v>21</v>
+      </c>
+      <c r="K83">
+        <v>4.5</v>
+      </c>
+      <c r="L83">
+        <v>39</v>
+      </c>
+      <c r="N83">
+        <v>122</v>
+      </c>
+      <c r="O83">
+        <v>7.03</v>
+      </c>
+      <c r="P83">
+        <v>4.25</v>
+      </c>
+      <c r="Q83">
+        <v>194</v>
+      </c>
+      <c r="R83">
+        <v>67.7</v>
+      </c>
+      <c r="S83">
+        <v>4</v>
+      </c>
+      <c r="T83">
+        <v>20</v>
+      </c>
+      <c r="W83">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:23">
+      <c r="A84" t="s">
+        <v>104</v>
+      </c>
+      <c r="B84">
+        <v>2018</v>
+      </c>
+      <c r="C84">
+        <v>21</v>
+      </c>
+      <c r="D84">
+        <v>175.26</v>
+      </c>
+      <c r="E84">
+        <v>86.18248</v>
+      </c>
+      <c r="F84">
+        <v>127</v>
+      </c>
+      <c r="G84">
+        <v>1226</v>
+      </c>
+      <c r="H84">
+        <v>9.653543307086615</v>
+      </c>
+      <c r="I84">
+        <v>4</v>
+      </c>
+      <c r="J84">
+        <v>39</v>
+      </c>
+      <c r="K84">
+        <v>4.53</v>
+      </c>
+      <c r="L84">
+        <v>34.5</v>
+      </c>
+      <c r="M84">
+        <v>13</v>
+      </c>
+      <c r="N84">
+        <v>113</v>
+      </c>
+      <c r="Q84">
+        <v>187</v>
+      </c>
+      <c r="R84">
+        <v>69.40000000000001</v>
+      </c>
+      <c r="S84">
+        <v>1.2</v>
+      </c>
+      <c r="T84">
+        <v>6</v>
+      </c>
+      <c r="W84">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:23">
+      <c r="A85" t="s">
+        <v>105</v>
+      </c>
+      <c r="B85">
+        <v>2018</v>
+      </c>
+      <c r="C85">
+        <v>22</v>
+      </c>
+      <c r="D85">
+        <v>187.96</v>
+      </c>
+      <c r="E85">
+        <v>91.625584</v>
+      </c>
+      <c r="F85">
+        <v>130</v>
+      </c>
+      <c r="G85">
+        <v>2040</v>
+      </c>
+      <c r="H85">
+        <v>15.69230769230769</v>
+      </c>
+      <c r="I85">
+        <v>20</v>
+      </c>
+      <c r="J85">
+        <v>40</v>
+      </c>
+      <c r="K85">
+        <v>4.43</v>
+      </c>
+      <c r="L85">
+        <v>33.5</v>
+      </c>
+      <c r="M85">
+        <v>11</v>
+      </c>
+      <c r="N85">
+        <v>115</v>
+      </c>
+      <c r="O85">
+        <v>6.71</v>
+      </c>
+      <c r="P85">
+        <v>4.37</v>
+      </c>
+      <c r="Q85">
+        <v>185</v>
+      </c>
+      <c r="R85">
+        <v>55.6</v>
+      </c>
+      <c r="S85">
+        <v>0.2</v>
+      </c>
+      <c r="T85">
+        <v>1</v>
+      </c>
+      <c r="W85">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:23">
+      <c r="A86" t="s">
+        <v>106</v>
+      </c>
+      <c r="B86">
+        <v>2018</v>
+      </c>
+      <c r="C86">
+        <v>23</v>
+      </c>
+      <c r="D86">
+        <v>193.04</v>
+      </c>
+      <c r="E86">
+        <v>93.43995200000001</v>
+      </c>
+      <c r="F86">
+        <v>119</v>
+      </c>
+      <c r="G86">
+        <v>1832</v>
+      </c>
+      <c r="H86">
+        <v>15.39495798319328</v>
+      </c>
+      <c r="I86">
+        <v>12</v>
+      </c>
+      <c r="J86">
+        <v>39</v>
+      </c>
+      <c r="K86">
+        <v>4.37</v>
+      </c>
+      <c r="L86">
+        <v>30.5</v>
+      </c>
+      <c r="M86">
+        <v>15</v>
+      </c>
+      <c r="N86">
+        <v>124</v>
+      </c>
+      <c r="Q86">
+        <v>174</v>
+      </c>
+      <c r="R86">
+        <v>62.6</v>
+      </c>
+      <c r="S86">
+        <v>4.8</v>
+      </c>
+      <c r="T86">
+        <v>24</v>
+      </c>
+      <c r="W86">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:23">
+      <c r="A87" t="s">
+        <v>107</v>
+      </c>
+      <c r="B87">
+        <v>2018</v>
+      </c>
+      <c r="C87">
+        <v>22</v>
+      </c>
+      <c r="D87">
+        <v>187.96</v>
+      </c>
+      <c r="E87">
+        <v>97.52227999999999</v>
+      </c>
+      <c r="F87">
+        <v>286</v>
+      </c>
+      <c r="G87">
+        <v>3777</v>
+      </c>
+      <c r="H87">
+        <v>13.20629370629371</v>
+      </c>
+      <c r="I87">
+        <v>33</v>
+      </c>
+      <c r="J87">
+        <v>40</v>
+      </c>
+      <c r="K87">
+        <v>4.44</v>
+      </c>
+      <c r="L87">
+        <v>40</v>
+      </c>
+      <c r="M87">
+        <v>20</v>
+      </c>
+      <c r="N87">
+        <v>124</v>
+      </c>
+      <c r="O87">
+        <v>7.08</v>
+      </c>
+      <c r="P87">
+        <v>4.26</v>
+      </c>
+      <c r="Q87">
+        <v>265</v>
+      </c>
+      <c r="R87">
+        <v>52.7</v>
+      </c>
+      <c r="S87">
+        <v>1</v>
+      </c>
+      <c r="T87">
+        <v>5</v>
+      </c>
+      <c r="W87">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:23">
+      <c r="A88" t="s">
+        <v>108</v>
+      </c>
+      <c r="B88">
+        <v>2018</v>
+      </c>
+      <c r="C88">
+        <v>22</v>
+      </c>
+      <c r="D88">
+        <v>195.58</v>
+      </c>
+      <c r="E88">
+        <v>102.965384</v>
+      </c>
+      <c r="F88">
+        <v>241</v>
+      </c>
+      <c r="G88">
+        <v>3360</v>
+      </c>
+      <c r="H88">
+        <v>13.94190871369295</v>
+      </c>
+      <c r="I88">
+        <v>26</v>
+      </c>
+      <c r="J88">
+        <v>48</v>
+      </c>
+      <c r="K88">
+        <v>4.55</v>
+      </c>
+      <c r="L88">
+        <v>38</v>
+      </c>
+      <c r="M88">
+        <v>17</v>
+      </c>
+      <c r="N88">
+        <v>122</v>
+      </c>
+      <c r="Q88">
+        <v>265</v>
+      </c>
+      <c r="R88">
+        <v>69</v>
+      </c>
+      <c r="S88">
+        <v>4.2</v>
+      </c>
+      <c r="T88">
+        <v>21</v>
+      </c>
+      <c r="W88">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W59">
-    <sortCondition ref="A2:A59"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>